<commit_message>
update fix error in J1C11 to J1B11
</commit_message>
<xml_diff>
--- a/A1 board IBM5100.xlsx
+++ b/A1 board IBM5100.xlsx
@@ -16572,6 +16572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17224,10 +17225,10 @@
       <c r="U6" s="14"/>
       <c r="V6" s="14"/>
       <c r="W6" s="14"/>
-      <c r="X6" s="24" t="s">
+      <c r="X6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="Y6" s="14"/>
+      <c r="Y6" s="13"/>
       <c r="Z6" s="14"/>
       <c r="AA6" s="14"/>
       <c r="AB6" s="14"/>
@@ -22718,6 +22719,9 @@
     <mergeCell ref="AF70:AJ70"/>
     <mergeCell ref="AK70:AO70"/>
   </mergeCells>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>